<commit_message>
Adding sequence data and correcting the species ID from Hillside Park
</commit_message>
<xml_diff>
--- a/Raw_data/site_list.xlsx
+++ b/Raw_data/site_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewsasaki/Desktop/Lab_Projects/diapt_ctmax_survey/Raw_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/msasaki/Desktop/Lab_Projects/diapt_ctmax_survey/Raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C439A56-0C24-6041-95FE-412D294517D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CCBFADE-98A0-1B45-AFD9-13225A434FA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{70252E7D-B877-DF4F-9713-FDF3EF035878}"/>
+    <workbookView xWindow="1220" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{70252E7D-B877-DF4F-9713-FDF3EF035878}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="61">
   <si>
     <t>site_num</t>
   </si>
@@ -59,9 +59,6 @@
     <t>collection_temp</t>
   </si>
   <si>
-    <t>Florida</t>
-  </si>
-  <si>
     <t>North Carolina</t>
   </si>
   <si>
@@ -104,9 +101,6 @@
     <t>OH</t>
   </si>
   <si>
-    <t>Green Lake</t>
-  </si>
-  <si>
     <t>Vermont</t>
   </si>
   <si>
@@ -140,28 +134,10 @@
     <t>Moosehead Lake</t>
   </si>
   <si>
-    <t>Lake Trafford</t>
-  </si>
-  <si>
-    <t>FL</t>
-  </si>
-  <si>
-    <t>Lake June</t>
-  </si>
-  <si>
-    <t>East Lake Tohopekaliga</t>
-  </si>
-  <si>
-    <t>Newnans Lake</t>
-  </si>
-  <si>
     <t>Ringneck Marsh</t>
   </si>
   <si>
     <t>Keuka Lake</t>
-  </si>
-  <si>
-    <t>Lake Eustis</t>
   </si>
   <si>
     <t>Lake Whalom</t>
@@ -651,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{681DA912-16C1-0D41-B94E-A4D9A4706D3F}">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="B15" sqref="B15:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -672,7 +648,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -698,13 +674,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="4">
         <v>44.511474</v>
@@ -718,13 +694,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" s="4">
         <v>44.595843000000002</v>
@@ -738,13 +714,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="4">
         <v>45.677449000000003</v>
@@ -758,13 +734,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="3">
         <v>45.910232999999998</v>
@@ -778,13 +754,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" s="3">
         <v>46.143495999999999</v>
@@ -798,13 +774,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" s="4">
         <v>46.671587000000002</v>
@@ -818,13 +794,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" s="3">
         <v>35.609053000000003</v>
@@ -844,13 +820,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" s="3">
         <v>35.7911644</v>
@@ -867,16 +843,16 @@
     </row>
     <row r="10" spans="1:8" ht="19">
       <c r="A10" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" s="6">
         <v>37.015326000000002</v>
@@ -893,16 +869,16 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E11" s="4">
         <v>37.750794999999997</v>
@@ -919,16 +895,16 @@
     </row>
     <row r="12" spans="1:8" ht="18">
       <c r="A12" s="1">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E12" s="3">
         <v>40.083305000000003</v>
@@ -945,16 +921,16 @@
     </row>
     <row r="13" spans="1:8" ht="18">
       <c r="A13" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E13" s="3">
         <v>41.486063999999999</v>
@@ -971,596 +947,473 @@
     </row>
     <row r="14" spans="1:8" ht="18">
       <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="E14" s="3">
+        <v>42.505361000000001</v>
+      </c>
+      <c r="F14" s="2">
+        <v>-74.975570000000005</v>
+      </c>
+      <c r="G14" s="5">
+        <v>45443</v>
+      </c>
+      <c r="H14" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="3">
-        <v>42.285623999999999</v>
-      </c>
-      <c r="F14" s="2">
-        <v>-73.884375000000006</v>
-      </c>
-      <c r="G14" s="5">
-        <v>45444</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="18">
-      <c r="A15" s="1">
-        <v>16</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="D15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="3">
-        <v>42.505361000000001</v>
+        <v>9</v>
+      </c>
+      <c r="E15" s="4">
+        <v>39.857290999999996</v>
       </c>
       <c r="F15" s="2">
-        <v>-74.975570000000005</v>
-      </c>
-      <c r="G15" s="5">
-        <v>45443</v>
-      </c>
-      <c r="H15" s="1">
-        <v>20</v>
+        <v>-83.022433000000007</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E16" s="4">
-        <v>39.857290999999996</v>
+        <v>41.597422999999999</v>
       </c>
       <c r="F16" s="2">
-        <v>-83.022433000000007</v>
+        <v>-80.538070000000005</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E17" s="4">
-        <v>41.597422999999999</v>
+        <v>42.402887</v>
       </c>
       <c r="F17" s="2">
-        <v>-80.538070000000005</v>
+        <v>-77.212911000000005</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E18" s="4">
-        <v>42.402887</v>
+        <v>43.139069999999997</v>
       </c>
       <c r="F18" s="2">
-        <v>-77.212911000000005</v>
+        <v>-78.381262000000007</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="E19" s="4">
-        <v>43.139069999999997</v>
+        <v>44.481127999999998</v>
       </c>
       <c r="F19" s="2">
-        <v>-78.381262000000007</v>
+        <v>-73.225581000000005</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E20" s="4">
-        <v>44.481127999999998</v>
+        <v>47.616047999999999</v>
       </c>
       <c r="F20" s="2">
-        <v>-73.225581000000005</v>
+        <v>-68.793222999999998</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E21" s="4">
-        <v>47.616047999999999</v>
+        <v>43.490426999999997</v>
       </c>
       <c r="F21" s="2">
-        <v>-68.793222999999998</v>
+        <v>-74.406566999999995</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E22" s="4">
-        <v>43.490426999999997</v>
+        <v>42.575761</v>
       </c>
       <c r="F22" s="2">
-        <v>-74.406566999999995</v>
+        <v>-71.744838000000001</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="4">
+        <v>42.465232999999998</v>
+      </c>
+      <c r="F23" s="2">
+        <v>-73.281081</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="18">
+      <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" s="4">
-        <v>42.575761</v>
-      </c>
-      <c r="F23" s="2">
-        <v>-71.744838000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="1">
+      <c r="B24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="3">
+        <v>42.464753999999999</v>
+      </c>
+      <c r="F24" s="2">
+        <v>-71.153582</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="4">
-        <v>42.465232999999998</v>
-      </c>
-      <c r="F24" s="2">
-        <v>-73.281081</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="18">
-      <c r="A25" s="1">
-        <v>25</v>
-      </c>
       <c r="B25" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="3">
-        <v>42.464753999999999</v>
+        <v>13</v>
+      </c>
+      <c r="E25" s="4">
+        <v>42.025022</v>
       </c>
       <c r="F25" s="2">
-        <v>-71.153582</v>
+        <v>-70.829712000000001</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E26" s="4">
-        <v>42.025022</v>
+        <v>41.775934999999997</v>
       </c>
       <c r="F26" s="2">
-        <v>-70.829712000000001</v>
+        <v>-72.528583999999995</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E27" s="4">
-        <v>41.775934999999997</v>
+        <v>41.953319999999998</v>
       </c>
       <c r="F27" s="2">
-        <v>-72.528583999999995</v>
+        <v>-71.900000000000006</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E28" s="4">
-        <v>41.953319999999998</v>
+        <v>41.501545</v>
       </c>
       <c r="F28" s="2">
-        <v>-71.900000000000006</v>
+        <v>-72.225506999999993</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E29" s="4">
-        <v>41.501545</v>
+        <v>41.342627</v>
       </c>
       <c r="F29" s="2">
-        <v>-72.225506999999993</v>
+        <v>-73.510311000000002</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E30" s="4">
-        <v>41.342627</v>
+        <v>42.934218999999999</v>
       </c>
       <c r="F30" s="2">
-        <v>-73.510311000000002</v>
+        <v>-73.790290999999996</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E31" s="4">
-        <v>42.934218999999999</v>
+        <v>42.878841000000001</v>
       </c>
       <c r="F31" s="2">
-        <v>-73.790290999999996</v>
+        <v>-75.574505000000002</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E32" s="4">
-        <v>42.878841000000001</v>
+        <v>42.450108999999998</v>
       </c>
       <c r="F32" s="2">
-        <v>-75.574505000000002</v>
+        <v>-75.058643000000004</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E33" s="4">
-        <v>42.450108999999998</v>
+        <v>41.217438000000001</v>
       </c>
       <c r="F33" s="2">
-        <v>-75.058643000000004</v>
+        <v>-74.298657000000006</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E34" s="4">
-        <v>41.217438000000001</v>
+        <v>42.100256000000002</v>
       </c>
       <c r="F34" s="2">
-        <v>-74.298657000000006</v>
+        <v>-78.739012000000002</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E35" s="4">
-        <v>42.100256000000002</v>
+        <v>41.158898000000001</v>
       </c>
       <c r="F35" s="2">
-        <v>-78.739012000000002</v>
+        <v>-78.841496000000006</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="1">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E36" s="4">
-        <v>41.158898000000001</v>
+        <v>41.011890999999999</v>
       </c>
       <c r="F36" s="2">
-        <v>-78.841496000000006</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="1">
-        <v>37</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E37" s="4">
-        <v>41.011890999999999</v>
-      </c>
-      <c r="F37" s="2">
         <v>-77.671019999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="1">
-        <v>7</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" s="4">
-        <v>26.432376999999999</v>
-      </c>
-      <c r="F41" s="2">
-        <v>-81.486333999999999</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="1">
-        <v>8</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E42" s="4">
-        <v>27.313123000000001</v>
-      </c>
-      <c r="F42" s="2">
-        <v>-81.371504000000002</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" s="1">
-        <v>9</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E43" s="4">
-        <v>28.26107</v>
-      </c>
-      <c r="F43" s="2">
-        <v>-81.284437999999994</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" s="1">
-        <v>10</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E44" s="4">
-        <v>28.857116000000001</v>
-      </c>
-      <c r="F44" s="2">
-        <v>-81.687734000000006</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" s="1">
-        <v>11</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E45" s="4">
-        <v>29.618074</v>
-      </c>
-      <c r="F45" s="2">
-        <v>-82.250645000000006</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H38">
-    <sortCondition ref="B1:B38"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H36">
+    <sortCondition ref="B1:B36"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Several batches of new experimental data
</commit_message>
<xml_diff>
--- a/Raw_data/site_list.xlsx
+++ b/Raw_data/site_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewsasaki/Desktop/Lab_Projects/diapt_ctmax_survey/Raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8C8D08-41EC-A34E-B1F2-5946793A4D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881D1374-417A-1945-BF10-397E8D0C5EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{70252E7D-B877-DF4F-9713-FDF3EF035878}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="66">
   <si>
     <t>site_num</t>
   </si>
@@ -140,9 +140,6 @@
     <t>Lake Onata</t>
   </si>
   <si>
-    <t>Stetson Pond</t>
-  </si>
-  <si>
     <t>Center Springs Pond</t>
   </si>
   <si>
@@ -221,10 +218,22 @@
     <t>Ashefield Lake</t>
   </si>
   <si>
-    <t>MA_C</t>
-  </si>
-  <si>
     <t>Cranberry Bog</t>
+  </si>
+  <si>
+    <t>Monponsett Pond</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>Fraser</t>
+  </si>
+  <si>
+    <t>Colorado</t>
+  </si>
+  <si>
+    <t>Grand Lake, CA</t>
   </si>
 </sst>
 </file>
@@ -621,10 +630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{681DA912-16C1-0D41-B94E-A4D9A4706D3F}">
-  <dimension ref="A1:M43"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="114" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -731,7 +740,7 @@
         <v>22</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>11</v>
@@ -794,7 +803,7 @@
         <v>17</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>7</v>
@@ -820,7 +829,7 @@
         <v>17</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>7</v>
@@ -846,7 +855,7 @@
         <v>17</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>8</v>
@@ -872,7 +881,7 @@
         <v>17</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>8</v>
@@ -898,7 +907,7 @@
         <v>17</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>12</v>
@@ -924,7 +933,7 @@
         <v>17</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>12</v>
@@ -950,7 +959,7 @@
         <v>17</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>15</v>
@@ -980,7 +989,7 @@
         <v>19</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>9</v>
@@ -1032,7 +1041,7 @@
         <v>19</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>15</v>
@@ -1058,7 +1067,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>12</v>
@@ -1127,7 +1136,7 @@
         <v>26</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>15</v>
@@ -1147,10 +1156,10 @@
         <v>21</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>13</v>
@@ -1173,7 +1182,7 @@
         <v>21</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>31</v>
@@ -1186,6 +1195,12 @@
       </c>
       <c r="F27" s="1">
         <v>-71.744838000000001</v>
+      </c>
+      <c r="G27" s="4">
+        <v>45470</v>
+      </c>
+      <c r="H27" s="3">
+        <v>24.5</v>
       </c>
     </row>
     <row r="28" spans="1:13">
@@ -1193,7 +1208,7 @@
         <v>22</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>33</v>
@@ -1213,10 +1228,10 @@
         <v>23</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>13</v>
@@ -1238,7 +1253,7 @@
         <v>23</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>32</v>
@@ -1258,33 +1273,39 @@
         <v>24</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E31" s="2">
-        <v>42.025022</v>
+        <v>42.006242999999998</v>
       </c>
       <c r="F31" s="1">
-        <v>-70.829712000000001</v>
+        <v>-70.841425999999998</v>
+      </c>
+      <c r="G31" s="4">
+        <v>45471</v>
+      </c>
+      <c r="H31" s="3">
+        <v>26.5</v>
       </c>
     </row>
     <row r="32" spans="1:13">
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:8">
       <c r="A33" s="3">
         <v>25</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>14</v>
@@ -1296,15 +1317,15 @@
         <v>-72.528583999999995</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:8">
       <c r="A34" s="3">
         <v>26</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>14</v>
@@ -1316,15 +1337,15 @@
         <v>-71.900000000000006</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:8">
       <c r="A35" s="3">
         <v>27</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>14</v>
@@ -1336,15 +1357,15 @@
         <v>-72.225506999999993</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:8">
       <c r="A36" s="3">
         <v>28</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>14</v>
@@ -1356,18 +1377,18 @@
         <v>-73.510311000000002</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:8">
       <c r="E37" s="2"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:8">
       <c r="A38" s="3">
         <v>29</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>15</v>
@@ -1379,15 +1400,15 @@
         <v>-73.790290999999996</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:8">
       <c r="A39" s="3">
         <v>30</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>15</v>
@@ -1399,15 +1420,15 @@
         <v>-75.574505000000002</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:8">
       <c r="A40" s="3">
         <v>31</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>15</v>
@@ -1419,15 +1440,15 @@
         <v>-75.058643000000004</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:8">
       <c r="A41" s="3">
         <v>32</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>15</v>
@@ -1439,15 +1460,15 @@
         <v>-74.298657000000006</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:8">
       <c r="A42" s="3">
         <v>33</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>12</v>
@@ -1459,15 +1480,15 @@
         <v>-78.841496000000006</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:8">
       <c r="A43" s="3">
         <v>34</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>12</v>
@@ -1477,6 +1498,58 @@
       </c>
       <c r="F43" s="1">
         <v>-77.671019999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="3">
+        <v>35</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E45" s="1">
+        <v>39.943925900000004</v>
+      </c>
+      <c r="F45" s="1">
+        <v>-105.810562</v>
+      </c>
+      <c r="G45" s="4">
+        <v>45489</v>
+      </c>
+      <c r="H45" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="3">
+        <v>36</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E46" s="1">
+        <v>40.250444000000002</v>
+      </c>
+      <c r="F46" s="1">
+        <v>-105.819607</v>
+      </c>
+      <c r="G46" s="4">
+        <v>45490</v>
+      </c>
+      <c r="H46" s="3">
+        <v>17.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>